<commit_message>
fix get dockercompose file
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,16 +433,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="46.8" customWidth="1" min="1" max="1"/>
     <col width="28.8" customWidth="1" min="2" max="2"/>
     <col width="39.6" customWidth="1" min="3" max="3"/>
     <col width="25.2" customWidth="1" min="4" max="4"/>
     <col width="31.2" customWidth="1" min="5" max="5"/>
-    <col width="10.8" customWidth="1" min="6" max="6"/>
+    <col width="15.6" customWidth="1" min="6" max="6"/>
     <col width="38.4" customWidth="1" min="7" max="7"/>
     <col width="19.2" customWidth="1" min="8" max="8"/>
     <col width="14.4" customWidth="1" min="9" max="9"/>
-    <col width="10.8" customWidth="1" min="10" max="10"/>
+    <col width="15.6" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,46 +500,258 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>alibghz/nestjs-microservices-docker</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>No CI/CD present</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Not</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>sqshq/piggymetrics</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Not present</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Not present</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>microservices touched by CI/CD</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Not present</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Not</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>aidanwhiteley/books</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No CI/CD present</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Not</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>alanjeffares/notebook-to-microservice</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No CI/CD present</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Not</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>aliyun/alibabacloud-microservice-demo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>microservices touched by CI/CD</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Not present</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Present</t>
         </is>

</xml_diff>